<commit_message>
excel reader product data
</commit_message>
<xml_diff>
--- a/src/main/java/easyexcel/product.xlsx
+++ b/src/main/java/easyexcel/product.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="32460" windowHeight="15000"/>
+    <workbookView windowWidth="30240" windowHeight="13420"/>
   </bookViews>
   <sheets>
     <sheet name="模板" sheetId="1" r:id="rId1"/>
@@ -27,11 +27,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>商品ID</t>
   </si>
   <si>
+    <t>关键属性-材质</t>
+  </si>
+  <si>
+    <t>关键属性-表面工艺</t>
+  </si>
+  <si>
+    <t>其它属性-材质</t>
+  </si>
+  <si>
     <t>商品规格-颜色</t>
   </si>
   <si>
@@ -41,6 +50,15 @@
     <t>6401218073696665600</t>
   </si>
   <si>
+    <t>亚克力</t>
+  </si>
+  <si>
+    <t>uv打印</t>
+  </si>
+  <si>
+    <t>金</t>
+  </si>
+  <si>
     <t>白</t>
   </si>
   <si>
@@ -51,6 +69,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
       <t>黑</t>
     </r>
     <r>
@@ -112,7 +135,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -129,6 +152,18 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF5A6C7D"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF5A6C7D"/>
+      <name val="宋体-简"/>
       <charset val="134"/>
     </font>
     <font>
@@ -614,28 +649,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -644,122 +670,131 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -767,7 +802,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1301,20 +1342,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="29.8076923076923" customWidth="1"/>
     <col min="2" max="2" width="28.3653846153846" customWidth="1"/>
-    <col min="3" max="3" width="20.8269230769231" customWidth="1"/>
+    <col min="3" max="3" width="31.4038461538462" customWidth="1"/>
+    <col min="4" max="4" width="28.3653846153846" customWidth="1"/>
+    <col min="5" max="5" width="26.9230769230769" customWidth="1"/>
+    <col min="6" max="6" width="35.2596153846154" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" spans="1:3">
+    <row r="1" ht="21" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,104 +1368,194 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" ht="17" spans="1:3">
+    <row r="3" ht="17" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" ht="17" spans="1:3">
+    <row r="4" ht="17" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" ht="17" spans="1:3">
+    <row r="5" ht="17" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" ht="17" spans="1:3">
+    <row r="6" ht="17" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="9" ht="17" spans="1:3">
+    <row r="9" ht="17" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="10" ht="17" spans="1:3">
+    <row r="10" ht="17" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>